<commit_message>
Fixed an error with the calibration source uncertainty
</commit_message>
<xml_diff>
--- a/Simulated/Activation/DetectorModel/Cs137Data.xlsx
+++ b/Simulated/Activation/DetectorModel/Cs137Data.xlsx
@@ -333,19 +333,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.6440879725641458E-5</c:v>
+                    <c:v>2.5121578195521086E-5</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.7180691077143448E-5</c:v>
+                    <c:v>2.5582728758372584E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.6719180821702987E-5</c:v>
+                    <c:v>2.5269281509228832E-5</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.6602620147657855E-5</c:v>
+                    <c:v>2.5153507616072824E-5</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.6438787582501609E-5</c:v>
+                    <c:v>2.506297721776219E-5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -357,19 +357,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.6440879725641458E-5</c:v>
+                    <c:v>2.5121578195521086E-5</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.7180691077143448E-5</c:v>
+                    <c:v>2.5582728758372584E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.6719180821702987E-5</c:v>
+                    <c:v>2.5269281509228832E-5</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.6602620147657855E-5</c:v>
+                    <c:v>2.5153507616072824E-5</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.6438787582501609E-5</c:v>
+                    <c:v>2.506297721776219E-5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -486,11 +486,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="422072144"/>
-        <c:axId val="422072536"/>
+        <c:axId val="500480056"/>
+        <c:axId val="500480448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="422072144"/>
+        <c:axId val="500480056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,12 +546,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422072536"/>
+        <c:crossAx val="500480448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="422072536"/>
+        <c:axId val="500480448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,7 +608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422072144"/>
+        <c:crossAx val="500480056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -783,19 +783,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>9.4359981502925008E-4</c:v>
+                    <c:v>4.9713441843073341E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6057028788690132E-3</c:v>
+                    <c:v>7.5091825786858775E-4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0141405728368677E-3</c:v>
+                    <c:v>5.3057717154343111E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0732042982709198E-3</c:v>
+                    <c:v>5.4927569179468718E-4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2442764650411491E-3</c:v>
+                    <c:v>6.1935085131089316E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -807,19 +807,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>9.4359981502925008E-4</c:v>
+                    <c:v>4.9713441843073341E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6057028788690132E-3</c:v>
+                    <c:v>7.5091825786858775E-4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0141405728368677E-3</c:v>
+                    <c:v>5.3057717154343111E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0732042982709198E-3</c:v>
+                    <c:v>5.4927569179468718E-4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2442764650411491E-3</c:v>
+                    <c:v>6.1935085131089316E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -982,11 +982,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="422073320"/>
-        <c:axId val="422073712"/>
+        <c:axId val="500481232"/>
+        <c:axId val="500481624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="422073320"/>
+        <c:axId val="500481232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,12 +1042,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422073712"/>
+        <c:crossAx val="500481624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="422073712"/>
+        <c:axId val="500481624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2.5000000000000005E-2"/>
@@ -1105,7 +1105,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422073320"/>
+        <c:crossAx val="500481232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2286,7 +2286,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B78C694-7289-435E-8A7F-823492F07C8E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5B78C694-7289-435E-8A7F-823492F07C8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2322,7 +2322,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D803B8BA-66BB-433A-B114-135A0E71F3CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D803B8BA-66BB-433A-B114-135A0E71F3CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2609,7 +2609,7 @@
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2771,8 +2771,8 @@
         <v>1.6292166551842952E-3</v>
       </c>
       <c r="P2" s="2">
-        <f>SQRT((N2/M2)^2+(0.01/L2^2)+0.02^2)*O2</f>
-        <v>3.6440879725641458E-5</v>
+        <f>SQRT((N2/M2)^2+(0.1/L2^2)+0.01165^2)*O2</f>
+        <v>2.5121578195521086E-5</v>
       </c>
       <c r="Q2" s="2">
         <v>1.6037E-3</v>
@@ -2783,15 +2783,15 @@
       </c>
       <c r="S2" s="2">
         <f>3*P2+O2</f>
-        <v>1.7385392943612195E-3</v>
+        <v>1.7045813897708585E-3</v>
       </c>
       <c r="T2" s="3">
         <f>0.97*Q2/S2</f>
-        <v>0.89476781171722675</v>
+        <v>0.91259297404925499</v>
       </c>
       <c r="U2" s="3">
         <f t="shared" ref="U2:U8" si="0">(O2-Q2)^2/P2^2</f>
-        <v>0.49030890858207027</v>
+        <v>1.0317005240977319</v>
       </c>
       <c r="V2" s="2">
         <v>7.3232000000000002E-3</v>
@@ -2861,8 +2861,8 @@
         <v>1.6596406035800258E-3</v>
       </c>
       <c r="P3" s="6">
-        <f t="shared" ref="P3:P11" si="5">SQRT((N3/M3)^2+(0.1/L3^2)+0.02^2)*O3</f>
-        <v>3.7180691077143448E-5</v>
+        <f>SQRT((N3/M3)^2+(0.1/L3^2)+0.01165^2)*O3</f>
+        <v>2.5582728758372584E-5</v>
       </c>
       <c r="Q3" s="6">
         <v>1.6167E-3</v>
@@ -2873,15 +2873,15 @@
       </c>
       <c r="S3" s="6">
         <f>3*P3+O3</f>
-        <v>1.7711826768114561E-3</v>
+        <v>1.7363887898551435E-3</v>
       </c>
       <c r="T3" s="7">
         <f>0.97*Q3/S3</f>
-        <v>0.88539653223298553</v>
+        <v>0.90313817341036018</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="0"/>
-        <v>1.3338327415794129</v>
+        <v>2.8173613785719183</v>
       </c>
       <c r="V3" s="6">
         <v>7.4644000000000004E-3</v>
@@ -2890,11 +2890,11 @@
         <v>37078</v>
       </c>
       <c r="X3" s="6">
-        <f t="shared" ref="X3:X11" si="6">(W3/L3)/(I3*C3)</f>
+        <f t="shared" ref="X3:X11" si="5">(W3/L3)/(I3*C3)</f>
         <v>6.1193470862709026E-3</v>
       </c>
       <c r="Y3" s="6">
-        <f t="shared" ref="Y3:Y11" si="7">V3/X3</f>
+        <f t="shared" ref="Y3:Y11" si="6">V3/X3</f>
         <v>1.219803337638226</v>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D6" si="8">30.07*365*24*3600</f>
+        <f t="shared" ref="D4:D6" si="7">30.07*365*24*3600</f>
         <v>948287519.99999988</v>
       </c>
       <c r="E4" s="1">
@@ -2923,7 +2923,7 @@
         <v>39814</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H6" si="9">(E4-G4)*24*3600</f>
+        <f t="shared" ref="H4:H6" si="8">(E4-G4)*24*3600</f>
         <v>259200000</v>
       </c>
       <c r="I4">
@@ -2951,8 +2951,8 @@
         <v>1.638800812638878E-3</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" si="5"/>
-        <v>3.6719180821702987E-5</v>
+        <f t="shared" ref="P4:P6" si="9">SQRT((N4/M4)^2+(0.1/L4^2)+0.01165^2)*O4</f>
+        <v>2.5269281509228832E-5</v>
       </c>
       <c r="Q4" s="2">
         <v>1.6027000000000001E-3</v>
@@ -2963,15 +2963,15 @@
       </c>
       <c r="S4" s="2">
         <f>3*P4+O4</f>
-        <v>1.7489583551039869E-3</v>
+        <v>1.7146086571665645E-3</v>
       </c>
       <c r="T4" s="3">
         <f t="shared" ref="T4:T11" si="10">0.97*Q4/S4</f>
-        <v>0.88888280013252119</v>
+        <v>0.90669027798392698</v>
       </c>
       <c r="U4" s="3">
         <f t="shared" si="0"/>
-        <v>0.96660266572601283</v>
+        <v>2.0410242697045895</v>
       </c>
       <c r="V4" s="2">
         <v>7.3026000000000002E-3</v>
@@ -2980,11 +2980,11 @@
         <v>42961</v>
       </c>
       <c r="X4" s="2">
+        <f t="shared" si="5"/>
+        <v>7.0148479760652454E-3</v>
+      </c>
+      <c r="Y4" s="2">
         <f t="shared" si="6"/>
-        <v>7.0148479760652454E-3</v>
-      </c>
-      <c r="Y4" s="2">
-        <f t="shared" si="7"/>
         <v>1.0410204219559096</v>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>948287519.99999988</v>
       </c>
       <c r="E5" s="5">
@@ -3013,7 +3013,7 @@
         <v>39814</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>259200000</v>
       </c>
       <c r="I5" s="4">
@@ -3041,8 +3041,8 @@
         <v>1.6356705923779825E-3</v>
       </c>
       <c r="P5" s="6">
-        <f t="shared" si="5"/>
-        <v>3.6602620147657855E-5</v>
+        <f t="shared" si="9"/>
+        <v>2.5153507616072824E-5</v>
       </c>
       <c r="Q5" s="6">
         <v>1.5705999999999999E-3</v>
@@ -3053,15 +3053,15 @@
       </c>
       <c r="S5" s="6">
         <f>3*P5+O5</f>
-        <v>1.745478452820956E-3</v>
+        <v>1.711131115226201E-3</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="10"/>
-        <v>0.87281627426441355</v>
+        <v>0.89033621470824864</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="0"/>
-        <v>3.1604226895846481</v>
+        <v>6.6922539120075735</v>
       </c>
       <c r="V5" s="6">
         <v>7.2798999999999997E-3</v>
@@ -3070,11 +3070,11 @@
         <v>38965</v>
       </c>
       <c r="X5" s="6">
+        <f t="shared" si="5"/>
+        <v>6.2679016779607294E-3</v>
+      </c>
+      <c r="Y5" s="6">
         <f t="shared" si="6"/>
-        <v>6.2679016779607294E-3</v>
-      </c>
-      <c r="Y5" s="6">
-        <f t="shared" si="7"/>
         <v>1.1614572745449518</v>
       </c>
     </row>
@@ -3089,7 +3089,7 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="D6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>948287519.99999988</v>
       </c>
       <c r="E6" s="1">
@@ -3103,7 +3103,7 @@
         <v>39814</v>
       </c>
       <c r="H6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>259200000</v>
       </c>
       <c r="I6">
@@ -3131,8 +3131,8 @@
         <v>1.6270648612971867E-3</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" si="5"/>
-        <v>3.6438787582501609E-5</v>
+        <f t="shared" si="9"/>
+        <v>2.506297721776219E-5</v>
       </c>
       <c r="Q6" s="2">
         <v>1.5923000000000001E-3</v>
@@ -3143,15 +3143,15 @@
       </c>
       <c r="S6" s="2">
         <f>3*P6+O6</f>
-        <v>1.7363812240446916E-3</v>
+        <v>1.7022537929504732E-3</v>
       </c>
       <c r="T6" s="3">
         <f t="shared" si="10"/>
-        <v>0.88951146131504488</v>
+        <v>0.90734472520863274</v>
       </c>
       <c r="U6" s="3">
         <f t="shared" si="0"/>
-        <v>0.91023423379316881</v>
+        <v>1.9240470296854428</v>
       </c>
       <c r="V6" s="2">
         <v>7.2759000000000001E-3</v>
@@ -3160,11 +3160,11 @@
         <v>38954</v>
       </c>
       <c r="X6" s="2">
+        <f t="shared" si="5"/>
+        <v>6.2825931630671791E-3</v>
+      </c>
+      <c r="Y6" s="2">
         <f t="shared" si="6"/>
-        <v>6.2825931630671791E-3</v>
-      </c>
-      <c r="Y6" s="2">
-        <f t="shared" si="7"/>
         <v>1.1581045933026619</v>
       </c>
     </row>
@@ -3221,8 +3221,8 @@
         <v>3.0297830356941006E-2</v>
       </c>
       <c r="P7" s="6">
-        <f t="shared" si="5"/>
-        <v>9.4359981502925008E-4</v>
+        <f>SQRT((N7/M7)^2+(0.01/L7^2)+0.01165^2)*O7</f>
+        <v>4.9713441843073341E-4</v>
       </c>
       <c r="Q7" s="6">
         <v>3.2863999999999997E-2</v>
@@ -3233,15 +3233,15 @@
       </c>
       <c r="S7" s="6">
         <f t="shared" ref="S7:S11" si="19">3*P7+O7</f>
-        <v>3.3128629802028756E-2</v>
+        <v>3.1789233612233209E-2</v>
       </c>
       <c r="T7" s="7">
         <f>0.97*Q7/S7</f>
-        <v>0.96225168956573692</v>
+        <v>1.0027948578078523</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="0"/>
-        <v>7.3959681468459832</v>
+        <v>26.645450189086791</v>
       </c>
       <c r="V7" s="6">
         <v>0.18402499999999999</v>
@@ -3250,11 +3250,11 @@
         <v>49230</v>
       </c>
       <c r="X7" s="6">
+        <f t="shared" si="5"/>
+        <v>0.12628692042708056</v>
+      </c>
+      <c r="Y7" s="6">
         <f t="shared" si="6"/>
-        <v>0.12628692042708056</v>
-      </c>
-      <c r="Y7" s="6">
-        <f t="shared" si="7"/>
         <v>1.4571976209227306</v>
       </c>
     </row>
@@ -3311,8 +3311,8 @@
         <v>4.1851898270809561E-2</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" si="5"/>
-        <v>1.6057028788690132E-3</v>
+        <f t="shared" ref="P8:P11" si="20">SQRT((N8/M8)^2+(0.01/L8^2)+0.01165^2)*O8</f>
+        <v>7.5091825786858775E-4</v>
       </c>
       <c r="Q8" s="2">
         <v>4.3739E-2</v>
@@ -3323,15 +3323,15 @@
       </c>
       <c r="S8" s="2">
         <f t="shared" si="19"/>
-        <v>4.6669006907416599E-2</v>
+        <v>4.4104653044415326E-2</v>
       </c>
       <c r="T8" s="3">
         <f>0.97*Q8/S8</f>
-        <v>0.9091007675429571</v>
+        <v>0.96195813981972189</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" si="0"/>
-        <v>1.381211714640614</v>
+        <v>6.315464486563088</v>
       </c>
       <c r="V8" s="2">
         <v>0.26486500000000002</v>
@@ -3340,11 +3340,11 @@
         <v>49121</v>
       </c>
       <c r="X8" s="2">
+        <f t="shared" si="5"/>
+        <v>0.17951041231546822</v>
+      </c>
+      <c r="Y8" s="2">
         <f t="shared" si="6"/>
-        <v>0.17951041231546822</v>
-      </c>
-      <c r="Y8" s="2">
-        <f t="shared" si="7"/>
         <v>1.4754854416719363</v>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" ref="D9:D11" si="20">30.07*365*24*3600</f>
+        <f t="shared" ref="D9:D11" si="21">30.07*365*24*3600</f>
         <v>948287519.99999988</v>
       </c>
       <c r="E9" s="5">
@@ -3401,8 +3401,8 @@
         <v>3.2818668584155629E-2</v>
       </c>
       <c r="P9" s="6">
-        <f t="shared" si="5"/>
-        <v>1.0141405728368677E-3</v>
+        <f t="shared" si="20"/>
+        <v>5.3057717154343111E-4</v>
       </c>
       <c r="Q9" s="6">
         <v>3.2815700000000003E-2</v>
@@ -3413,15 +3413,15 @@
       </c>
       <c r="S9" s="6">
         <f t="shared" si="19"/>
-        <v>3.5861090302666231E-2</v>
+        <v>3.4410400098785925E-2</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" si="10"/>
-        <v>0.88762580087068321</v>
+        <v>0.92504675646369716</v>
       </c>
       <c r="U9" s="7">
-        <f t="shared" ref="U9:U11" si="21">(O9-Q9)^2/P9^2</f>
-        <v>8.5684529121661486E-6</v>
+        <f t="shared" ref="U9:U11" si="22">(O9-Q9)^2/P9^2</f>
+        <v>3.1304127938176428E-5</v>
       </c>
       <c r="V9" s="6">
         <v>0.18431500000000001</v>
@@ -3430,11 +3430,11 @@
         <v>49476</v>
       </c>
       <c r="X9" s="6">
+        <f t="shared" si="5"/>
+        <v>0.12586616385951582</v>
+      </c>
+      <c r="Y9" s="6">
         <f t="shared" si="6"/>
-        <v>0.12586616385951582</v>
-      </c>
-      <c r="Y9" s="6">
-        <f t="shared" si="7"/>
         <v>1.4643729049033483</v>
       </c>
     </row>
@@ -3449,29 +3449,29 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="D10" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>948287519.99999988</v>
       </c>
       <c r="E10" s="1">
         <v>42814</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F11" si="22">K10*37000</f>
+        <f t="shared" ref="F10:F11" si="23">K10*37000</f>
         <v>38554</v>
       </c>
       <c r="G10" s="1">
         <v>39814</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H11" si="23">(E10-G10)*24*3600</f>
+        <f t="shared" ref="H10:H11" si="24">(E10-G10)*24*3600</f>
         <v>259200000</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I11" si="24">F10*EXP(-J10*H10)</f>
+        <f t="shared" ref="I10:I11" si="25">F10*EXP(-J10*H10)</f>
         <v>31899.763472592538</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10:J11" si="25">LN(2)/D10</f>
+        <f t="shared" ref="J10:J11" si="26">LN(2)/D10</f>
         <v>7.3094622247052809E-10</v>
       </c>
       <c r="K10">
@@ -3491,8 +3491,8 @@
         <v>3.2796098698359658E-2</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="5"/>
-        <v>1.0732042982709198E-3</v>
+        <f t="shared" si="20"/>
+        <v>5.4927569179468718E-4</v>
       </c>
       <c r="Q10" s="2">
         <v>3.2927699999999997E-2</v>
@@ -3503,15 +3503,15 @@
       </c>
       <c r="S10" s="2">
         <f t="shared" si="19"/>
-        <v>3.601571159317242E-2</v>
+        <v>3.4443925773743722E-2</v>
       </c>
       <c r="T10" s="3">
         <f t="shared" si="10"/>
-        <v>0.88683154065613157</v>
+        <v>0.92730048281393795</v>
       </c>
       <c r="U10" s="3">
-        <f t="shared" si="21"/>
-        <v>1.5036804830212474E-2</v>
+        <f t="shared" si="22"/>
+        <v>5.740366352774974E-2</v>
       </c>
       <c r="V10" s="2">
         <v>0.18396000000000001</v>
@@ -3520,11 +3520,11 @@
         <v>49733</v>
       </c>
       <c r="X10" s="2">
+        <f t="shared" si="5"/>
+        <v>0.14006186038586893</v>
+      </c>
+      <c r="Y10" s="2">
         <f t="shared" si="6"/>
-        <v>0.14006186038586893</v>
-      </c>
-      <c r="Y10" s="2">
-        <f t="shared" si="7"/>
         <v>1.3134196525249071</v>
       </c>
     </row>
@@ -3539,29 +3539,29 @@
         <v>0.85099999999999998</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>948287519.99999988</v>
       </c>
       <c r="E11" s="5">
         <v>42814</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>38554</v>
       </c>
       <c r="G11" s="5">
         <v>39814</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>259200000</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>31899.763472592538</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>7.3094622247052809E-10</v>
       </c>
       <c r="K11" s="4">
@@ -3581,8 +3581,8 @@
         <v>3.6693035189762045E-2</v>
       </c>
       <c r="P11" s="6">
-        <f t="shared" si="5"/>
-        <v>1.2442764650411491E-3</v>
+        <f t="shared" si="20"/>
+        <v>6.1935085131089316E-4</v>
       </c>
       <c r="Q11" s="6">
         <v>3.27893E-2</v>
@@ -3593,15 +3593,15 @@
       </c>
       <c r="S11" s="6">
         <f t="shared" si="19"/>
-        <v>4.0425864584885493E-2</v>
+        <v>3.8551087743694722E-2</v>
       </c>
       <c r="T11" s="7">
         <f t="shared" si="10"/>
-        <v>0.7867641502933137</v>
+        <v>0.82502525509677771</v>
       </c>
       <c r="U11" s="7">
-        <f t="shared" si="21"/>
-        <v>9.8429873228299094</v>
+        <f t="shared" si="22"/>
+        <v>39.727132734181616</v>
       </c>
       <c r="V11" s="6">
         <v>0.18412300000000001</v>
@@ -3610,18 +3610,18 @@
         <v>50210</v>
       </c>
       <c r="X11" s="6">
+        <f t="shared" si="5"/>
+        <v>0.15110950418119387</v>
+      </c>
+      <c r="Y11" s="6">
         <f t="shared" si="6"/>
-        <v>0.15110950418119387</v>
-      </c>
-      <c r="Y11" s="6">
-        <f t="shared" si="7"/>
         <v>1.2184739867799446</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="U12" s="12">
         <f>SUM(U2:U11)/9</f>
-        <v>2.8329570885405491</v>
+        <v>9.6946521657282698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>